<commit_message>
fixed logo on captains contacts
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -669,15 +669,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2225405</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -701,8 +701,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="19050" y="95249"/>
-          <a:ext cx="2066924" cy="1343025"/>
+          <a:off x="123825" y="257174"/>
+          <a:ext cx="2101580" cy="971551"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A42" sqref="A1:D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SW fixed captains list, club roster, team captain lists,junior girls,zone 3 4, beat the champ
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="-165" windowWidth="24915" windowHeight="12600"/>
+    <workbookView xWindow="900" yWindow="1110" windowWidth="24915" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$43</definedName>
+  </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="152">
   <si>
     <t>WOMEN’S ZONE 4 CLUB ROSTER</t>
   </si>
   <si>
-    <t>CAPTAIN’S LIST</t>
-  </si>
-  <si>
     <t>Beach Grove</t>
   </si>
   <si>
@@ -180,9 +180,6 @@
     <t>jlouchang@gmail.com</t>
   </si>
   <si>
-    <t>McCleery Tuesday</t>
-  </si>
-  <si>
     <t>Christine Hoag</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>dchoag@shaw.ca</t>
   </si>
   <si>
-    <t>Mylora Thursday</t>
-  </si>
-  <si>
     <t>Kathie Patterson</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>scooterlady@telus.net</t>
   </si>
   <si>
-    <t>Mylora Tuesday</t>
-  </si>
-  <si>
     <t>Esther Caldes</t>
   </si>
   <si>
@@ -216,9 +207,6 @@
     <t>esthercaldes@gmail.com</t>
   </si>
   <si>
-    <t>Mylora Saturday</t>
-  </si>
-  <si>
     <t>Musqueam</t>
   </si>
   <si>
@@ -390,27 +378,6 @@
     <t>Club</t>
   </si>
   <si>
-    <t>2018 Captain</t>
-  </si>
-  <si>
-    <t>Fraserview Business Women</t>
-  </si>
-  <si>
-    <t>Fraserview Tuesday</t>
-  </si>
-  <si>
-    <t>Kings Links Business Women</t>
-  </si>
-  <si>
-    <t>McCleery Business Women</t>
-  </si>
-  <si>
-    <t>Tsawwassen Springs Business Women</t>
-  </si>
-  <si>
-    <t>University Business Women</t>
-  </si>
-  <si>
     <t>Brenda Nordgren</t>
   </si>
   <si>
@@ -454,6 +421,60 @@
   </si>
   <si>
     <t xml:space="preserve">Telephone </t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>2018 CAPTAIN’S LIST</t>
+  </si>
+  <si>
+    <t>Business Women</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Fraserview</t>
+  </si>
+  <si>
+    <t>604-536-6204</t>
+  </si>
+  <si>
+    <t>lillymoe48@gmail.com</t>
+  </si>
+  <si>
+    <t>Lillian Moe</t>
+  </si>
+  <si>
+    <t>* Playing on</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Mylora</t>
+  </si>
+  <si>
+    <t>Sandy Heatherington</t>
+  </si>
+  <si>
+    <t>Rhiannon Charles</t>
+  </si>
+  <si>
+    <t>marinedrive.bizwomen@gmail.com</t>
+  </si>
+  <si>
+    <t>McCleery</t>
+  </si>
+  <si>
+    <t>Tsawwassen</t>
+  </si>
+  <si>
+    <t>* Business Women play on the weekend but some may play weekday evening</t>
   </si>
 </sst>
 </file>
@@ -484,8 +505,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -506,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -545,19 +566,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -601,53 +609,264 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -669,15 +888,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>219616</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2225405</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>120379</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -687,7 +906,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -701,8 +920,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="123825" y="257174"/>
-          <a:ext cx="2101580" cy="971551"/>
+          <a:off x="219616" y="114300"/>
+          <a:ext cx="1091388" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1011,571 +1230,661 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="33"/>
+      <c r="B1" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-    </row>
-    <row r="4" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="E13" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="38"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="B27" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+      <c r="B28" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="42"/>
+      <c r="B29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="E34" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C38" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="21" t="s">
+      <c r="C39" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B38" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="E39" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="7" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="42"/>
+      <c r="B40" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B39" s="7" t="s">
+      <c r="D40" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="E41" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="7" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="B42" s="27"/>
+      <c r="C42" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="D42" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="E42" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>117</v>
+    </row>
+    <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
+  <mergeCells count="13">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.4" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
SW removed marine drive BW
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="149">
   <si>
     <t>WOMEN’S ZONE 4 CLUB ROSTER</t>
   </si>
@@ -457,15 +457,6 @@
   </si>
   <si>
     <t>Mylora</t>
-  </si>
-  <si>
-    <t>Sandy Heatherington</t>
-  </si>
-  <si>
-    <t>Rhiannon Charles</t>
-  </si>
-  <si>
-    <t>marinedrive.bizwomen@gmail.com</t>
   </si>
   <si>
     <t>McCleery</t>
@@ -527,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -712,19 +703,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -767,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -816,57 +794,45 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1230,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A19" sqref="A19:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,31 +1212,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1395,7 +1361,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="31" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1412,7 +1378,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="7" t="s">
         <v>136</v>
       </c>
@@ -1457,7 +1423,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1474,7 +1440,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
@@ -1504,10 +1470,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="34" t="s">
         <v>137</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -1521,8 +1487,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="10" t="s">
         <v>115</v>
       </c>
@@ -1532,357 +1498,332 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="38"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>51</v>
+        <v>124</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>136</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="7"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="C26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="7" t="s">
-        <v>143</v>
-      </c>
+      <c r="A28" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="7"/>
       <c r="C28" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>129</v>
+      <c r="A29" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B30" s="7"/>
-      <c r="C30" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>69</v>
+      <c r="C30" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="15" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="15" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="15" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="15" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="15" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>90</v>
+        <v>147</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>94</v>
+      <c r="A37" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>150</v>
-      </c>
+      <c r="A38" s="32"/>
       <c r="B38" s="7" t="s">
         <v>136</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="A39" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="4"/>
       <c r="C39" s="5" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28" t="s">
+      <c r="B40" s="27"/>
+      <c r="C40" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D40" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="E42" s="29" t="s">
+      <c r="E40" s="29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
-        <v>151</v>
+    <row r="41" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
+  <mergeCells count="10">
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.4" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SW email links not working in pdf
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -763,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -795,20 +795,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -816,10 +809,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -850,8 +850,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1216,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A1:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,12 +1283,12 @@
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
@@ -1299,12 +1298,12 @@
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7"/>
@@ -1314,12 +1313,12 @@
       <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="7"/>
@@ -1329,12 +1328,12 @@
       <c r="D8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="8"/>
@@ -1344,12 +1343,12 @@
       <c r="D9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="7"/>
@@ -1359,12 +1358,12 @@
       <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="7"/>
@@ -1374,7 +1373,7 @@
       <c r="D11" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="26" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1391,7 +1390,7 @@
       <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1406,7 +1405,7 @@
       <c r="D13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="26" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1421,12 +1420,12 @@
       <c r="D14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="26" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="7"/>
@@ -1436,7 +1435,7 @@
       <c r="D15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1453,7 +1452,7 @@
       <c r="D16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="26" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1468,12 +1467,12 @@
       <c r="D17" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="26" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="7"/>
@@ -1483,7 +1482,7 @@
       <c r="D18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="26" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1497,10 +1496,10 @@
       <c r="C19" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="26" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1511,12 +1510,12 @@
         <v>115</v>
       </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="7"/>
@@ -1526,7 +1525,7 @@
       <c r="D21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="26" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1543,7 +1542,7 @@
       <c r="D22" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1558,12 +1557,12 @@
       <c r="D23" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="26" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="7"/>
@@ -1573,7 +1572,7 @@
       <c r="D24" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="26" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1590,7 +1589,7 @@
       <c r="D25" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="26" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1605,7 +1604,7 @@
       <c r="D26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="26" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1620,12 +1619,12 @@
       <c r="D27" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="28" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B28" s="7"/>
@@ -1635,12 +1634,12 @@
       <c r="D28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="26" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="18" t="s">
         <v>70</v>
       </c>
       <c r="B29" s="7"/>
@@ -1650,12 +1649,12 @@
       <c r="D29" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="25" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="18" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="7"/>
@@ -1665,12 +1664,12 @@
       <c r="D30" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="25" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="18" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="7"/>
@@ -1680,12 +1679,12 @@
       <c r="D31" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="25" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="18" t="s">
         <v>82</v>
       </c>
       <c r="B32" s="7"/>
@@ -1695,12 +1694,12 @@
       <c r="D32" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="25" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="18" t="s">
         <v>83</v>
       </c>
       <c r="B33" s="7"/>
@@ -1710,12 +1709,12 @@
       <c r="D33" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="25" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="18" t="s">
         <v>87</v>
       </c>
       <c r="B34" s="7"/>
@@ -1725,12 +1724,12 @@
       <c r="D34" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="25" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B35" s="7"/>
@@ -1740,7 +1739,7 @@
       <c r="D35" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="25" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1754,10 +1753,10 @@
       <c r="C36" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E36" s="25" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1772,7 +1771,7 @@
       <c r="D37" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="26" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1789,7 +1788,7 @@
       <c r="D38" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="26" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1804,12 +1803,12 @@
       <c r="D39" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="26" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="17" t="s">
         <v>105</v>
       </c>
       <c r="B40" s="4"/>
@@ -1819,27 +1818,27 @@
       <c r="D40" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="26" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27" t="s">
+      <c r="B41" s="21"/>
+      <c r="C41" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="29" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="23" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1860,10 +1859,46 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E36" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
+    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="E12" r:id="rId7"/>
+    <hyperlink ref="E13" r:id="rId8"/>
+    <hyperlink ref="E14" r:id="rId9"/>
+    <hyperlink ref="E15" r:id="rId10"/>
+    <hyperlink ref="E16" r:id="rId11"/>
+    <hyperlink ref="E17" r:id="rId12"/>
+    <hyperlink ref="E18" r:id="rId13"/>
+    <hyperlink ref="E19" r:id="rId14"/>
+    <hyperlink ref="E20" r:id="rId15"/>
+    <hyperlink ref="E21" r:id="rId16"/>
+    <hyperlink ref="E22" r:id="rId17"/>
+    <hyperlink ref="E23" r:id="rId18"/>
+    <hyperlink ref="E24" r:id="rId19"/>
+    <hyperlink ref="E25" r:id="rId20"/>
+    <hyperlink ref="E26" r:id="rId21"/>
+    <hyperlink ref="E27" r:id="rId22"/>
+    <hyperlink ref="E28" r:id="rId23"/>
+    <hyperlink ref="E29" r:id="rId24"/>
+    <hyperlink ref="E30" r:id="rId25"/>
+    <hyperlink ref="E31" r:id="rId26"/>
+    <hyperlink ref="E32" r:id="rId27"/>
+    <hyperlink ref="E33" r:id="rId28"/>
+    <hyperlink ref="E34" r:id="rId29"/>
+    <hyperlink ref="E35" r:id="rId30"/>
+    <hyperlink ref="E37" r:id="rId31"/>
+    <hyperlink ref="E38" r:id="rId32"/>
+    <hyperlink ref="E39" r:id="rId33"/>
+    <hyperlink ref="E40" r:id="rId34"/>
+    <hyperlink ref="E41" r:id="rId35"/>
+    <hyperlink ref="E5" r:id="rId36"/>
+    <hyperlink ref="E6" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.4" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
+  <drawing r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SW added Ladies Tee Golf Club
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="2490" windowWidth="24915" windowHeight="12600"/>
+    <workbookView xWindow="1515" yWindow="720" windowWidth="24915" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$43</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
   <si>
     <t>WOMEN’S ZONE 4 CLUB ROSTER</t>
   </si>
@@ -475,6 +475,18 @@
   </si>
   <si>
     <t>mundick2@telus.net</t>
+  </si>
+  <si>
+    <t>Ladies Tee Golf Club</t>
+  </si>
+  <si>
+    <t>Marg Masuch</t>
+  </si>
+  <si>
+    <t>604-916-0696</t>
+  </si>
+  <si>
+    <t>margmacsuch@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -763,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -820,6 +832,31 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -829,35 +866,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1213,15 +1256,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A1:E42"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
@@ -1229,31 +1272,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="39" t="s">
+      <c r="A1" s="34"/>
+      <c r="B1" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="38" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1283,7 +1326,7 @@
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="31" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1378,7 +1421,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="39" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1395,7 +1438,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="7" t="s">
         <v>136</v>
       </c>
@@ -1440,7 +1483,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1457,7 +1500,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
@@ -1472,393 +1515,408 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>41</v>
+      <c r="A18" s="30" t="s">
+        <v>152</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E19" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E20" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="10" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="28" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="5" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E22" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E23" s="26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="12" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
+      <c r="B24" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E24" s="26" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E25" s="26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="26" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E26" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E27" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="2" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
+      <c r="B28" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C28" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E28" s="28" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B29" s="7"/>
-      <c r="C29" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>73</v>
+      <c r="C29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="15" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="15" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D36" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E36" s="25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C37" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D37" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E37" s="25" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="7" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="40"/>
+      <c r="B38" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E38" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E39" s="26" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="7" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="40"/>
+      <c r="B40" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E40" s="26" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E41" s="26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="22" t="s">
+      <c r="B42" s="21"/>
+      <c r="C42" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D42" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="E42" s="29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+    <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
         <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E36" r:id="rId1"/>
+    <hyperlink ref="E37" r:id="rId1"/>
     <hyperlink ref="E7" r:id="rId2"/>
     <hyperlink ref="E8" r:id="rId3"/>
     <hyperlink ref="E9" r:id="rId4"/>
@@ -1870,35 +1928,36 @@
     <hyperlink ref="E15" r:id="rId10"/>
     <hyperlink ref="E16" r:id="rId11"/>
     <hyperlink ref="E17" r:id="rId12"/>
-    <hyperlink ref="E18" r:id="rId13"/>
-    <hyperlink ref="E19" r:id="rId14"/>
-    <hyperlink ref="E20" r:id="rId15"/>
-    <hyperlink ref="E21" r:id="rId16"/>
-    <hyperlink ref="E22" r:id="rId17"/>
-    <hyperlink ref="E23" r:id="rId18"/>
-    <hyperlink ref="E24" r:id="rId19"/>
-    <hyperlink ref="E25" r:id="rId20"/>
-    <hyperlink ref="E26" r:id="rId21"/>
-    <hyperlink ref="E27" r:id="rId22"/>
-    <hyperlink ref="E28" r:id="rId23"/>
-    <hyperlink ref="E29" r:id="rId24"/>
-    <hyperlink ref="E30" r:id="rId25"/>
-    <hyperlink ref="E31" r:id="rId26"/>
-    <hyperlink ref="E32" r:id="rId27"/>
-    <hyperlink ref="E33" r:id="rId28"/>
-    <hyperlink ref="E34" r:id="rId29"/>
-    <hyperlink ref="E35" r:id="rId30"/>
-    <hyperlink ref="E37" r:id="rId31"/>
-    <hyperlink ref="E38" r:id="rId32"/>
-    <hyperlink ref="E39" r:id="rId33"/>
-    <hyperlink ref="E40" r:id="rId34"/>
-    <hyperlink ref="E41" r:id="rId35"/>
+    <hyperlink ref="E19" r:id="rId13"/>
+    <hyperlink ref="E20" r:id="rId14"/>
+    <hyperlink ref="E21" r:id="rId15"/>
+    <hyperlink ref="E22" r:id="rId16"/>
+    <hyperlink ref="E23" r:id="rId17"/>
+    <hyperlink ref="E24" r:id="rId18"/>
+    <hyperlink ref="E25" r:id="rId19"/>
+    <hyperlink ref="E26" r:id="rId20"/>
+    <hyperlink ref="E27" r:id="rId21"/>
+    <hyperlink ref="E28" r:id="rId22"/>
+    <hyperlink ref="E29" r:id="rId23"/>
+    <hyperlink ref="E30" r:id="rId24"/>
+    <hyperlink ref="E31" r:id="rId25"/>
+    <hyperlink ref="E32" r:id="rId26"/>
+    <hyperlink ref="E33" r:id="rId27"/>
+    <hyperlink ref="E34" r:id="rId28"/>
+    <hyperlink ref="E35" r:id="rId29"/>
+    <hyperlink ref="E36" r:id="rId30"/>
+    <hyperlink ref="E38" r:id="rId31"/>
+    <hyperlink ref="E39" r:id="rId32"/>
+    <hyperlink ref="E40" r:id="rId33"/>
+    <hyperlink ref="E41" r:id="rId34"/>
+    <hyperlink ref="E42" r:id="rId35"/>
     <hyperlink ref="E5" r:id="rId36"/>
     <hyperlink ref="E6" r:id="rId37"/>
+    <hyperlink ref="E18" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.4" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
-  <drawing r:id="rId39"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
+  <drawing r:id="rId40"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SW dianmcneely new email
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -216,9 +216,6 @@
     <t>604-620-9470</t>
   </si>
   <si>
-    <t>dianemcneely@shaw.ca</t>
-  </si>
-  <si>
     <t>Pender Harbour</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>margmacsuch@gmail.com</t>
+  </si>
+  <si>
+    <t>dianemcneely8@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -836,6 +836,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -856,15 +865,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,47 +1272,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,21 +1411,21 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="E11" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>138</v>
+      <c r="A12" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>26</v>
@@ -1438,18 +1438,18 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="26" t="s">
         <v>122</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,11 +1483,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="32" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>38</v>
@@ -1500,33 +1500,33 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="26" t="s">
         <v>139</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="26" t="s">
         <v>154</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,14 +1545,14 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>137</v>
+      <c r="B20" s="35" t="s">
+        <v>136</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>46</v>
@@ -1562,10 +1562,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="28" t="s">
@@ -1588,11 +1588,11 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
-        <v>146</v>
+      <c r="A23" s="32" t="s">
+        <v>145</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>53</v>
@@ -1605,18 +1605,18 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="26" t="s">
         <v>125</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,15 +1631,15 @@
         <v>64</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>145</v>
+      <c r="A26" s="32" t="s">
+        <v>144</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>59</v>
@@ -1652,9 +1652,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>56</v>
@@ -1667,253 +1667,253 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="28" t="s">
         <v>128</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="26" t="s">
         <v>68</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="E30" s="25" t="s">
         <v>72</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="E31" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="E32" s="25" t="s">
         <v>80</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="E33" s="25" t="s">
         <v>131</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="E34" s="25" t="s">
         <v>85</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="E35" s="25" t="s">
         <v>89</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="E36" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="25" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="7" t="s">
+      <c r="D38" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="C39" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E39" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="26" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="33"/>
+      <c r="B40" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="26" t="s">
         <v>103</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="E41" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="E42" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E37" r:id="rId1"/>

</xml_diff>

<commit_message>
SW updated an email
</commit_message>
<xml_diff>
--- a/secure/captains_contact2018.xlsx
+++ b/secure/captains_contact2018.xlsx
@@ -300,9 +300,6 @@
     <t>604-740-1826</t>
   </si>
   <si>
-    <t>bd2006@telus.net</t>
-  </si>
-  <si>
     <t>Moira Milligan</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>dianemcneely8@gmail.com</t>
+  </si>
+  <si>
+    <t>bevdrombolis@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -836,6 +836,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -844,27 +865,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,47 +1272,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="39" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,21 +1411,21 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="E11" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>137</v>
+      <c r="A12" s="39" t="s">
+        <v>136</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>26</v>
@@ -1438,18 +1438,18 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,11 +1483,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>38</v>
@@ -1500,33 +1500,33 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="26" t="s">
         <v>138</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="26" t="s">
         <v>153</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,14 +1545,14 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="35" t="s">
-        <v>136</v>
+      <c r="B20" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>46</v>
@@ -1562,10 +1562,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="28" t="s">
@@ -1588,11 +1588,11 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>145</v>
+      <c r="A23" s="39" t="s">
+        <v>144</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>53</v>
@@ -1605,18 +1605,18 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="26" t="s">
         <v>124</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,15 +1631,15 @@
         <v>64</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>144</v>
+      <c r="A26" s="39" t="s">
+        <v>143</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>59</v>
@@ -1652,9 +1652,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>56</v>
@@ -1667,18 +1667,18 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="28" t="s">
         <v>127</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1747,13 +1747,13 @@
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="E33" s="25" t="s">
         <v>130</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,122 +1798,122 @@
         <v>92</v>
       </c>
       <c r="E36" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="40"/>
+      <c r="B38" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="7" t="s">
+      <c r="D38" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="C39" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E39" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="26" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="40"/>
+      <c r="B40" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="26" t="s">
         <v>102</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="E41" s="26" t="s">
         <v>106</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="E42" s="29" t="s">
         <v>110</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E37" r:id="rId1"/>

</xml_diff>